<commit_message>
Make validation and database logic for data prestasi and berkas ktmse gakin
</commit_message>
<xml_diff>
--- a/exports/xlsx/data_pendaftar.xlsx
+++ b/exports/xlsx/data_pendaftar.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Data Pribadi" sheetId="1" r:id="rId4"/>
     <sheet name="Data Sekolah" sheetId="2" r:id="rId5"/>
     <sheet name="Program Studi" sheetId="3" r:id="rId6"/>
+    <sheet name="Data Prestasi" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
   <si>
     <t>No.</t>
   </si>
@@ -58,49 +59,49 @@
     <t>Jalur Pendaftaran</t>
   </si>
   <si>
+    <t>Aditiya Ramadhan Saputra</t>
+  </si>
+  <si>
+    <t>Jalan Tanah Mas Azhar Blok C4 No4 Talang Kelapa, Kabputen Banyuasin, Suamatera Selatan</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>081271718692</t>
+  </si>
+  <si>
+    <t>Pria</t>
+  </si>
+  <si>
+    <t>Sukajadi</t>
+  </si>
+  <si>
+    <t>2001-11-20</t>
+  </si>
+  <si>
+    <t>pas_foto_001.jpg</t>
+  </si>
+  <si>
+    <t>PMDP</t>
+  </si>
+  <si>
     <t>Muhammad Naufal Kateni</t>
   </si>
   <si>
-    <t>Jl. M. P. Mangkunegara Komp. Tirta Kencana Blok C.5 Palembang, Indonesia</t>
-  </si>
-  <si>
-    <t>001</t>
+    <t>Jl. M. P. Mangkunegara Komp. Tirta Kencana Blok C5, Palembang, Sumatera Selatan</t>
+  </si>
+  <si>
+    <t>002</t>
   </si>
   <si>
     <t>0816382001</t>
   </si>
   <si>
-    <t>Pria</t>
-  </si>
-  <si>
     <t>Palembang</t>
   </si>
   <si>
-    <t>0021-11-25</t>
-  </si>
-  <si>
-    <t>pas_foto_001.jpg</t>
-  </si>
-  <si>
-    <t>pmdp</t>
-  </si>
-  <si>
-    <t>Aditiya Ramadhan Saputra</t>
-  </si>
-  <si>
-    <t>Talang Kelapa</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>0123456789</t>
-  </si>
-  <si>
-    <t>Banyuasin</t>
-  </si>
-  <si>
-    <t>2001-11-20</t>
+    <t>2001-11-25</t>
   </si>
   <si>
     <t>pas_foto_002.jpg</t>
@@ -115,7 +116,7 @@
     <t>003</t>
   </si>
   <si>
-    <t>0123456788</t>
+    <t>0895620677790</t>
   </si>
   <si>
     <t>2001-06-12</t>
@@ -175,31 +176,31 @@
     <t>IPA</t>
   </si>
   <si>
+    <t>SMAN 1 Talang Kelapa</t>
+  </si>
+  <si>
+    <t>Negeri</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>rekap_nilai_rapot_001.xlsx</t>
+  </si>
+  <si>
     <t>SMAS Kusuma Bangsa Palembang</t>
   </si>
   <si>
     <t>Swasta</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>rekap_nilai_rapot_001.pdf</t>
-  </si>
-  <si>
-    <t>SMAN 1 Talang Kelapa</t>
-  </si>
-  <si>
-    <t>Negeri</t>
-  </si>
-  <si>
-    <t>rekap_nilai_rapot_002.pdf</t>
+    <t>rekap_nilai_rapot_002.xlsx</t>
   </si>
   <si>
     <t>SMAN 18 Palembang</t>
   </si>
   <si>
-    <t>rekap_nilai_rapot_003.pdf</t>
+    <t>rekap_nilai_rapot_003.xlsx</t>
   </si>
   <si>
     <t>Bukti Pembayaran</t>
@@ -214,19 +215,43 @@
     <t>bukti_pembayaran_001.jpg</t>
   </si>
   <si>
-    <t>DIII Farmasi</t>
-  </si>
-  <si>
-    <t>--Lewati jika hanya membayar 1 pilihan--</t>
+    <t>Prodi DIII Farmasi</t>
   </si>
   <si>
     <t>bukti_pembayaran_002.jpg</t>
   </si>
   <si>
+    <t>Prodi DIII Teknologi Laboratorium Medis (TLM)</t>
+  </si>
+  <si>
     <t>bukti_pembayaran_003.jpg</t>
   </si>
   <si>
-    <t>DIII Gizi Palembang</t>
+    <t>Prestasi 1</t>
+  </si>
+  <si>
+    <t>Prestasi 2</t>
+  </si>
+  <si>
+    <t>Prestasi 3</t>
+  </si>
+  <si>
+    <t>Prestasi 4</t>
+  </si>
+  <si>
+    <t>Prestasi 5</t>
+  </si>
+  <si>
+    <t>prestasi_1_001.pdf</t>
+  </si>
+  <si>
+    <t>prestasi_2_001.pdf</t>
+  </si>
+  <si>
+    <t>prestasi_3_001.pdf</t>
+  </si>
+  <si>
+    <t>prestasi_1_003.pdf</t>
   </si>
 </sst>
 </file>
@@ -625,7 +650,7 @@
         <v>14</v>
       </c>
       <c r="D2">
-        <v>30163</v>
+        <v>30961</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -637,10 +662,10 @@
         <v>17</v>
       </c>
       <c r="H2">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="I2">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -666,7 +691,7 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>30111</v>
+        <v>30163</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -725,7 +750,7 @@
         <v>70</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="K4" t="s">
         <v>33</v>
@@ -842,19 +867,19 @@
         <v>16</v>
       </c>
       <c r="H2">
-        <v>1671</v>
+        <v>1607</v>
       </c>
       <c r="I2" t="s">
         <v>54</v>
       </c>
       <c r="J2">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="K2" t="s">
         <v>55</v>
       </c>
       <c r="L2">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -895,19 +920,19 @@
         <v>16</v>
       </c>
       <c r="H3">
-        <v>1607</v>
+        <v>1671</v>
       </c>
       <c r="I3" t="s">
         <v>54</v>
       </c>
       <c r="J3">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="K3" t="s">
         <v>58</v>
       </c>
       <c r="L3">
-        <v>90</v>
+        <v>90.5</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -942,7 +967,7 @@
         <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G4">
         <v>16</v>
@@ -954,13 +979,13 @@
         <v>54</v>
       </c>
       <c r="J4">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="K4" t="s">
         <v>60</v>
       </c>
       <c r="L4">
-        <v>90</v>
+        <v>95.8</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -1037,9 +1062,7 @@
       <c r="D2" t="s">
         <v>65</v>
       </c>
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
+      <c r="E2"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
@@ -1049,13 +1072,13 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
         <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1069,11 +1092,108 @@
         <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>69</v>
       </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2"/>
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>